<commit_message>
Consistent region codes: BALT, NAtl, NSEA, LDF, MBS
</commit_message>
<xml_diff>
--- a/Metiers/Reference_lists/RDB_ISSG_Metier_level5_list.xlsx
+++ b/Metiers/Reference_lists/RDB_ISSG_Metier_level5_list.xlsx
@@ -359,9 +359,6 @@
     <t>FPO_SPF_&gt;0_0_0</t>
   </si>
   <si>
-    <t>BS</t>
-  </si>
-  <si>
     <t>LLD_ANA_0_0_0</t>
   </si>
   <si>
@@ -666,6 +663,9 @@
   </si>
   <si>
     <t>SV_FIF</t>
+  </si>
+  <si>
+    <t>BALT</t>
   </si>
 </sst>
 </file>
@@ -1417,8 +1417,8 @@
   <dimension ref="A1:G235"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K124" sqref="K124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,27 +1437,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>160</v>
-      </c>
       <c r="G1" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>LEFT(G2,7)</f>
@@ -1472,10 +1472,10 @@
         <v>MOL</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F2" s="46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="60" t="s">
         <v>8</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B3" s="1" t="str">
         <f>LEFT(G3,7)</f>
@@ -1498,10 +1498,10 @@
         <v>MOL</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G3" s="48" t="s">
         <v>8</v>
@@ -1509,7 +1509,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="1" t="str">
         <f>LEFT(G4,7)</f>
@@ -1524,10 +1524,10 @@
         <v>MOL</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="40" t="s">
         <v>8</v>
@@ -1538,27 +1538,27 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>166</v>
-      </c>
       <c r="F5" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G5" s="48" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>110</v>
+      <c r="A6" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>LEFT(G6,7)</f>
@@ -1573,18 +1573,18 @@
         <v>ANA</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G6" s="61" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>110</v>
+      <c r="A7" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>LEFT(G7,7)</f>
@@ -1599,10 +1599,10 @@
         <v>CAT</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G7" s="61" t="s">
         <v>78</v>
@@ -1613,27 +1613,27 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G8" s="48" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>110</v>
+      <c r="A9" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B9" s="1" t="str">
         <f>LEFT(G9,7)</f>
@@ -1648,10 +1648,10 @@
         <v>CRU</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G9" s="61" t="s">
         <v>79</v>
@@ -1662,27 +1662,27 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G10" s="48" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>110</v>
+      <c r="A11" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" ref="B11:B42" si="0">LEFT(G11,7)</f>
@@ -1697,18 +1697,18 @@
         <v>DEF</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F11" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G11" s="61" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>110</v>
+      <c r="A12" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1723,10 +1723,10 @@
         <v>FWS</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G12" s="61" t="s">
         <v>104</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1749,10 +1749,10 @@
         <v>LPF</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G13" s="40" t="s">
         <v>2</v>
@@ -1760,7 +1760,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1775,10 +1775,10 @@
         <v>LPF</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G14" s="48" t="s">
         <v>2</v>
@@ -1801,18 +1801,18 @@
         <v>MOL</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G15" s="48" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>110</v>
+      <c r="A16" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1827,18 +1827,18 @@
         <v>SPF</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F16" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G16" s="61" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>110</v>
+      <c r="A17" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1853,18 +1853,18 @@
         <v>ANA</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F17" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G17" s="61" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>110</v>
+      <c r="A18" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1879,10 +1879,10 @@
         <v>CAT</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F18" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G18" s="61" t="s">
         <v>102</v>
@@ -1890,7 +1890,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1905,18 +1905,18 @@
         <v>CAT</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G19" s="40" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>110</v>
+      <c r="A20" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1931,10 +1931,10 @@
         <v>CRU</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F20" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G20" s="61" t="s">
         <v>3</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1957,18 +1957,18 @@
         <v>CRU</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1983,10 +1983,10 @@
         <v>CRU</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G22" s="48" t="s">
         <v>3</v>
@@ -1994,7 +1994,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2009,10 +2009,10 @@
         <v>CRU</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G23" s="40" t="s">
         <v>3</v>
@@ -2035,18 +2035,18 @@
         <v>CRU</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G24" s="48" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>110</v>
+      <c r="A25" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2061,10 +2061,10 @@
         <v>DEF</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G25" s="61" t="s">
         <v>82</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2087,10 +2087,10 @@
         <v>DEF</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G26" s="48" t="s">
         <v>82</v>
@@ -2098,7 +2098,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B27" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2113,10 +2113,10 @@
         <v>FIF</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G27" s="40" t="s">
         <v>4</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B28" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2139,10 +2139,10 @@
         <v>FIF</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G28" s="40" t="s">
         <v>4</v>
@@ -2165,18 +2165,18 @@
         <v>FIF</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G29" s="48" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>110</v>
+      <c r="A30" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B30" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2191,18 +2191,18 @@
         <v>FWS</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F30" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G30" s="61" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>110</v>
+      <c r="A31" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B31" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2217,10 +2217,10 @@
         <v>MOL</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F31" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G31" s="61" t="s">
         <v>5</v>
@@ -2228,7 +2228,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B32" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2243,10 +2243,10 @@
         <v>MOL</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G32" s="40" t="s">
         <v>5</v>
@@ -2269,18 +2269,18 @@
         <v>MOL</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G33" s="48" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
-        <v>110</v>
+      <c r="A34" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B34" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2295,18 +2295,18 @@
         <v>SPF</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F34" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G34" s="61" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>110</v>
+      <c r="A35" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B35" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2321,18 +2321,18 @@
         <v>ANA</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F35" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G35" s="61" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>110</v>
+      <c r="A36" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B36" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2347,10 +2347,10 @@
         <v>CAT</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F36" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G36" s="61" t="s">
         <v>6</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B37" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2373,10 +2373,10 @@
         <v>CAT</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G37" s="48" t="s">
         <v>6</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2399,10 +2399,10 @@
         <v>CAT</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G38" s="40" t="s">
         <v>6</v>
@@ -2425,18 +2425,18 @@
         <v>CAT</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G39" s="48" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
-        <v>110</v>
+      <c r="A40" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B40" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2451,10 +2451,10 @@
         <v>DEF</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F40" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G40" s="61" t="s">
         <v>7</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B41" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2477,10 +2477,10 @@
         <v>DEF</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G41" s="48" t="s">
         <v>7</v>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B42" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2503,10 +2503,10 @@
         <v>DEF</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G42" s="40" t="s">
         <v>7</v>
@@ -2529,18 +2529,18 @@
         <v>DEF</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G43" s="48" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
-        <v>110</v>
+      <c r="A44" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B44" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2555,18 +2555,18 @@
         <v>FWS</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F44" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G44" s="61" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
-        <v>110</v>
+      <c r="A45" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B45" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2581,18 +2581,18 @@
         <v>SPF</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F45" s="47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G45" s="61" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
-        <v>110</v>
+      <c r="A46" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B46" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2607,18 +2607,18 @@
         <v>ANA</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G46" s="45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B47" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2633,10 +2633,10 @@
         <v>DEF</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G47" s="26" t="s">
         <v>83</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B48" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2659,10 +2659,10 @@
         <v>DEF</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G48" s="32" t="s">
         <v>9</v>
@@ -2685,10 +2685,10 @@
         <v>DEF</v>
       </c>
       <c r="E49" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G49" s="50" t="s">
         <v>9</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B50" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2711,10 +2711,10 @@
         <v>SPF</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G50" s="26" t="s">
         <v>84</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B51" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2737,10 +2737,10 @@
         <v>SPF</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G51" s="32" t="s">
         <v>10</v>
@@ -2763,18 +2763,18 @@
         <v>SPF</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G52" s="50" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
-        <v>110</v>
+      <c r="A53" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B53" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2789,18 +2789,18 @@
         <v>ANA</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G53" s="45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="25" t="s">
-        <v>110</v>
+      <c r="A54" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B54" s="5" t="str">
         <f t="shared" si="3"/>
@@ -2815,18 +2815,18 @@
         <v>CAT</v>
       </c>
       <c r="E54" s="75" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F54" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G54" s="79" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B55" s="4" t="str">
         <f t="shared" si="3"/>
@@ -2841,18 +2841,18 @@
         <v>CAT</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F55" s="53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G55" s="72" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="s">
-        <v>110</v>
+      <c r="A56" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B56" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2867,10 +2867,10 @@
         <v>CRU</v>
       </c>
       <c r="E56" s="76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F56" s="67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G56" s="45" t="s">
         <v>11</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B57" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2893,10 +2893,10 @@
         <v>CRU</v>
       </c>
       <c r="E57" s="53" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F57" s="53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G57" s="32" t="s">
         <v>12</v>
@@ -2919,18 +2919,18 @@
         <v>CRU</v>
       </c>
       <c r="E58" s="77" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F58" s="78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G58" s="50" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
-        <v>110</v>
+      <c r="A59" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B59" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2945,18 +2945,18 @@
         <v>DEF</v>
       </c>
       <c r="E59" s="76" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F59" s="67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G59" s="45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2971,10 +2971,10 @@
         <v>DEF</v>
       </c>
       <c r="E60" s="69" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F60" s="69" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G60" s="26" t="s">
         <v>85</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B61" s="1" t="str">
         <f t="shared" si="3"/>
@@ -2997,10 +2997,10 @@
         <v>DEF</v>
       </c>
       <c r="E61" s="53" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F61" s="53" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G61" s="32" t="s">
         <v>13</v>
@@ -3023,10 +3023,10 @@
         <v>DEF</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G62" s="50" t="s">
         <v>13</v>
@@ -3034,7 +3034,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B63" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3049,18 +3049,18 @@
         <v>DWS</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G63" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="24" t="s">
-        <v>110</v>
+      <c r="A64" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B64" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3075,18 +3075,18 @@
         <v>FWS</v>
       </c>
       <c r="E64" s="76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F64" s="67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G64" s="45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B65" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3101,18 +3101,18 @@
         <v>SLP</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G65" s="26" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
-        <v>110</v>
+      <c r="A66" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B66" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3127,18 +3127,18 @@
         <v>SPF</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G66" s="45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B67" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3153,10 +3153,10 @@
         <v>SPF</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G67" s="32" t="s">
         <v>15</v>
@@ -3179,18 +3179,18 @@
         <v>SPF</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G68" s="50" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="24" t="s">
-        <v>110</v>
+      <c r="A69" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B69" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3205,18 +3205,18 @@
         <v>CAT</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G69" s="45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="24" t="s">
-        <v>110</v>
+      <c r="A70" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B70" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3231,18 +3231,18 @@
         <v>DEF</v>
       </c>
       <c r="E70" s="76" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F70" s="67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G70" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B71" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3257,10 +3257,10 @@
         <v>DEF</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G71" s="26" t="s">
         <v>87</v>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B72" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3283,10 +3283,10 @@
         <v>DEF</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G72" s="34" t="s">
         <v>16</v>
@@ -3309,18 +3309,18 @@
         <v>DEF</v>
       </c>
       <c r="E73" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G73" s="50" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="24" t="s">
-        <v>110</v>
+      <c r="A74" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B74" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3335,25 +3335,25 @@
         <v>FWS</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G74" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
-        <v>110</v>
+      <c r="A75" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B75" s="1" t="str">
         <f t="shared" si="3"/>
         <v>GTR_SPF</v>
       </c>
       <c r="C75" s="1" t="str">
-        <f t="shared" ref="C75:C106" si="6">LEFT(B75,3)</f>
+        <f t="shared" ref="C75:C77" si="6">LEFT(B75,3)</f>
         <v>GTR</v>
       </c>
       <c r="D75" s="1" t="str">
@@ -3361,18 +3361,18 @@
         <v>SPF</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G75" s="45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B76" s="1" t="str">
         <f t="shared" si="3"/>
@@ -3387,10 +3387,10 @@
         <v>MOL</v>
       </c>
       <c r="E76" s="68" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F76" s="71" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G76" s="27" t="s">
         <v>17</v>
@@ -3413,10 +3413,10 @@
         <v>MOL</v>
       </c>
       <c r="E77" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G77" s="40" t="s">
         <v>17</v>
@@ -3424,22 +3424,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="E78" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G78" s="29" t="s">
         <v>88</v>
@@ -3447,22 +3447,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="E79" s="3">
         <v>0</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G79" s="38" t="s">
         <v>89</v>
@@ -3470,22 +3470,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E80" s="3">
         <v>0</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G80" s="38" t="s">
         <v>90</v>
@@ -3493,7 +3493,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B81" s="1" t="str">
         <f t="shared" ref="B81:B112" si="7">LEFT(G81,7)</f>
@@ -3508,10 +3508,10 @@
         <v>CEP</v>
       </c>
       <c r="E81" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G81" s="55" t="s">
         <v>41</v>
@@ -3519,7 +3519,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B82" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3534,10 +3534,10 @@
         <v>DWS</v>
       </c>
       <c r="E82" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G82" s="55" t="s">
         <v>42</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B83" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3560,10 +3560,10 @@
         <v>FIF</v>
       </c>
       <c r="E83" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G83" s="55" t="s">
         <v>43</v>
@@ -3589,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G84" s="28" t="s">
         <v>43</v>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B85" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3612,10 +3612,10 @@
         <v>LPF</v>
       </c>
       <c r="E85" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F85" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G85" s="55" t="s">
         <v>18</v>
@@ -3623,7 +3623,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B86" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3638,10 +3638,10 @@
         <v>SPF</v>
       </c>
       <c r="E86" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G86" s="55" t="s">
         <v>44</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B87" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3664,10 +3664,10 @@
         <v>CEP</v>
       </c>
       <c r="E87" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F87" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G87" s="55" t="s">
         <v>19</v>
@@ -3693,15 +3693,15 @@
         <v>0</v>
       </c>
       <c r="F88" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G88" s="28" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="24" t="s">
-        <v>110</v>
+      <c r="A89" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B89" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3716,10 +3716,10 @@
         <v>FIF</v>
       </c>
       <c r="E89" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G89" s="63" t="s">
         <v>20</v>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B90" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3742,10 +3742,10 @@
         <v>FIF</v>
       </c>
       <c r="E90" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G90" s="55" t="s">
         <v>20</v>
@@ -3753,7 +3753,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B91" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3768,10 +3768,10 @@
         <v>FIF</v>
       </c>
       <c r="E91" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G91" s="55" t="s">
         <v>20</v>
@@ -3797,7 +3797,7 @@
         <v>0</v>
       </c>
       <c r="F92" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G92" s="28" t="s">
         <v>20</v>
@@ -3805,7 +3805,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B93" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3820,10 +3820,10 @@
         <v>LPF</v>
       </c>
       <c r="E93" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F93" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G93" s="55" t="s">
         <v>21</v>
@@ -3831,7 +3831,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B94" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3846,18 +3846,18 @@
         <v>MOL</v>
       </c>
       <c r="E94" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G94" s="55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B95" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3872,13 +3872,13 @@
         <v>SPF</v>
       </c>
       <c r="E95" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G95" s="55" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -3901,15 +3901,15 @@
         <v>0</v>
       </c>
       <c r="F96" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G96" s="28" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="24" t="s">
-        <v>110</v>
+      <c r="A97" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B97" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3924,18 +3924,18 @@
         <v>ANA</v>
       </c>
       <c r="E97" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G97" s="63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B98" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3950,18 +3950,18 @@
         <v>DWF</v>
       </c>
       <c r="E98" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F98" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G98" s="55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B99" s="1" t="str">
         <f t="shared" si="7"/>
@@ -3976,18 +3976,18 @@
         <v>DWS</v>
       </c>
       <c r="E99" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F99" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G99" s="55" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="24" t="s">
-        <v>110</v>
+      <c r="A100" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B100" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4002,10 +4002,10 @@
         <v>FIF</v>
       </c>
       <c r="E100" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G100" s="63" t="s">
         <v>26</v>
@@ -4013,7 +4013,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B101" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4028,10 +4028,10 @@
         <v>FIF</v>
       </c>
       <c r="E101" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G101" s="55" t="s">
         <v>26</v>
@@ -4057,7 +4057,7 @@
         <v>0</v>
       </c>
       <c r="F102" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G102" s="28" t="s">
         <v>26</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B103" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4080,10 +4080,10 @@
         <v>LPF</v>
       </c>
       <c r="E103" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F103" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G103" s="55" t="s">
         <v>23</v>
@@ -4091,7 +4091,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B104" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4109,7 +4109,7 @@
         <v>0</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G104" s="38" t="s">
         <v>23</v>
@@ -4117,7 +4117,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B105" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4132,10 +4132,10 @@
         <v>LPF</v>
       </c>
       <c r="E105" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F105" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G105" s="55" t="s">
         <v>23</v>
@@ -4161,15 +4161,15 @@
         <v>0</v>
       </c>
       <c r="F106" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G106" s="28" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="24" t="s">
-        <v>110</v>
+      <c r="A107" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B107" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4184,18 +4184,18 @@
         <v>SPF</v>
       </c>
       <c r="E107" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G107" s="63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B108" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4210,18 +4210,18 @@
         <v>SPF</v>
       </c>
       <c r="E108" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F108" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G108" s="55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="24" t="s">
-        <v>110</v>
+      <c r="A109" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B109" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4236,18 +4236,18 @@
         <v>ANA</v>
       </c>
       <c r="E109" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G109" s="63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="24" t="s">
-        <v>110</v>
+      <c r="A110" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B110" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4262,18 +4262,18 @@
         <v>CAT</v>
       </c>
       <c r="E110" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G110" s="63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B111" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4288,10 +4288,10 @@
         <v>DEF</v>
       </c>
       <c r="E111" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G111" s="55" t="s">
         <v>45</v>
@@ -4299,7 +4299,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B112" s="1" t="str">
         <f t="shared" si="7"/>
@@ -4314,10 +4314,10 @@
         <v>DWS</v>
       </c>
       <c r="E112" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G112" s="55" t="s">
         <v>24</v>
@@ -4343,15 +4343,15 @@
         <v>0</v>
       </c>
       <c r="F113" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G113" s="28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="24" t="s">
-        <v>110</v>
+      <c r="A114" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B114" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4366,10 +4366,10 @@
         <v>FIF</v>
       </c>
       <c r="E114" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G114" s="63" t="s">
         <v>27</v>
@@ -4377,7 +4377,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B115" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4392,10 +4392,10 @@
         <v>FIF</v>
       </c>
       <c r="E115" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F115" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G115" s="55" t="s">
         <v>27</v>
@@ -4403,7 +4403,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B116" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4421,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G116" s="38" t="s">
         <v>27</v>
@@ -4429,7 +4429,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B117" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4444,10 +4444,10 @@
         <v>FIF</v>
       </c>
       <c r="E117" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G117" s="55" t="s">
         <v>27</v>
@@ -4473,7 +4473,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="64" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G118" s="81" t="s">
         <v>27</v>
@@ -4481,7 +4481,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="23" t="s">
-        <v>110</v>
+        <v>212</v>
       </c>
       <c r="B119" s="4" t="str">
         <f t="shared" si="10"/>
@@ -4496,18 +4496,18 @@
         <v>FWS</v>
       </c>
       <c r="E119" s="66" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F119" s="65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G119" s="74" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B120" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4522,18 +4522,18 @@
         <v>MOL</v>
       </c>
       <c r="E120" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F120" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G120" s="55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="24" t="s">
-        <v>110</v>
+      <c r="A121" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B121" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4548,18 +4548,18 @@
         <v>SPF</v>
       </c>
       <c r="E121" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G121" s="63" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B122" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4574,18 +4574,18 @@
         <v>SPF</v>
       </c>
       <c r="E122" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F122" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G122" s="55" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B123" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4600,10 +4600,10 @@
         <v>LPF</v>
       </c>
       <c r="E123" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G123" s="55" t="s">
         <v>25</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B124" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4629,7 +4629,7 @@
         <v>0</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G124" s="38" t="s">
         <v>25</v>
@@ -4637,7 +4637,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B125" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4652,10 +4652,10 @@
         <v>LPF</v>
       </c>
       <c r="E125" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F125" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G125" s="55" t="s">
         <v>25</v>
@@ -4681,7 +4681,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G126" s="28" t="s">
         <v>25</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B127" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4704,18 +4704,18 @@
         <v>DEF</v>
       </c>
       <c r="E127" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F127" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G127" s="55" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B128" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4730,18 +4730,18 @@
         <v>DES</v>
       </c>
       <c r="E128" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G128" s="55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B129" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4756,18 +4756,18 @@
         <v>FIF</v>
       </c>
       <c r="E129" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G129" s="55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B130" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4782,18 +4782,18 @@
         <v>LPF</v>
       </c>
       <c r="E130" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G130" s="55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="24" t="s">
-        <v>110</v>
+      <c r="A131" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B131" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4808,10 +4808,10 @@
         <v>MIS</v>
       </c>
       <c r="E131" s="62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G131" s="63" t="s">
         <v>28</v>
@@ -4819,7 +4819,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B132" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4837,7 +4837,7 @@
         <v>0</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G132" s="38" t="s">
         <v>28</v>
@@ -4845,7 +4845,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B133" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4860,10 +4860,10 @@
         <v>MIS</v>
       </c>
       <c r="E133" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G133" s="55" t="s">
         <v>28</v>
@@ -4889,7 +4889,7 @@
         <v>0</v>
       </c>
       <c r="F134" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G134" s="28" t="s">
         <v>28</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B135" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4912,18 +4912,18 @@
         <v>MOL</v>
       </c>
       <c r="E135" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F135" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G135" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B136" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4938,18 +4938,18 @@
         <v>SPF</v>
       </c>
       <c r="E136" s="54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F136" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G136" s="55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B137" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4964,18 +4964,18 @@
         <v>CEP</v>
       </c>
       <c r="E137" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G137" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="24" t="s">
-        <v>110</v>
+      <c r="A138" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B138" s="1" t="str">
         <f t="shared" si="10"/>
@@ -4990,10 +4990,10 @@
         <v>CRU</v>
       </c>
       <c r="E138" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G138" s="32" t="s">
         <v>29</v>
@@ -5001,7 +5001,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B139" s="1" t="str">
         <f t="shared" si="10"/>
@@ -5016,10 +5016,10 @@
         <v>CRU</v>
       </c>
       <c r="E139" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G139" s="35" t="s">
         <v>47</v>
@@ -5027,7 +5027,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B140" s="1" t="str">
         <f t="shared" si="10"/>
@@ -5042,10 +5042,10 @@
         <v>CRU</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G140" s="35" t="s">
         <v>46</v>
@@ -5068,18 +5068,18 @@
         <v>CRU</v>
       </c>
       <c r="E141" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F141" s="42" t="s">
         <v>172</v>
-      </c>
-      <c r="F141" s="42" t="s">
-        <v>173</v>
       </c>
       <c r="G141" s="29" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A142" s="24" t="s">
-        <v>110</v>
+      <c r="A142" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B142" s="1" t="str">
         <f t="shared" si="10"/>
@@ -5094,10 +5094,10 @@
         <v>DEF</v>
       </c>
       <c r="E142" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F142" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G142" s="32" t="s">
         <v>30</v>
@@ -5105,7 +5105,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B143" s="1" t="str">
         <f t="shared" si="10"/>
@@ -5120,10 +5120,10 @@
         <v>DEF</v>
       </c>
       <c r="E143" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G143" s="35" t="s">
         <v>48</v>
@@ -5131,7 +5131,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B144" s="1" t="str">
         <f t="shared" si="10"/>
@@ -5146,10 +5146,10 @@
         <v>DEF</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F144" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G144" s="49" t="s">
         <v>91</v>
@@ -5157,7 +5157,7 @@
     </row>
     <row r="145" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B145" s="5" t="str">
         <f t="shared" ref="B145:B176" si="13">LEFT(G145,7)</f>
@@ -5172,10 +5172,10 @@
         <v>DEF</v>
       </c>
       <c r="E145" s="37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F145" s="37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G145" s="44" t="s">
         <v>30</v>
@@ -5198,10 +5198,10 @@
         <v>DEF</v>
       </c>
       <c r="E146" s="67" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F146" s="70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G146" s="80" t="s">
         <v>30</v>
@@ -5209,7 +5209,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B147" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5224,10 +5224,10 @@
         <v>DWS</v>
       </c>
       <c r="E147" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F147" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G147" s="49" t="s">
         <v>92</v>
@@ -5235,7 +5235,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B148" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5250,10 +5250,10 @@
         <v>DWS</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G148" s="35" t="s">
         <v>49</v>
@@ -5276,18 +5276,18 @@
         <v>DWS</v>
       </c>
       <c r="E149" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F149" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G149" s="29" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="24" t="s">
-        <v>110</v>
+      <c r="A150" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B150" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5302,18 +5302,18 @@
         <v>FWS</v>
       </c>
       <c r="E150" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G150" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B151" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5328,10 +5328,10 @@
         <v>MCD</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G151" s="35" t="s">
         <v>51</v>
@@ -5354,10 +5354,10 @@
         <v>MCD</v>
       </c>
       <c r="E152" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F152" s="42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G152" s="29" t="s">
         <v>52</v>
@@ -5365,7 +5365,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B153" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5380,10 +5380,10 @@
         <v>MCF</v>
       </c>
       <c r="E153" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G153" s="35" t="s">
         <v>54</v>
@@ -5391,7 +5391,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B154" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5406,10 +5406,10 @@
         <v>MCF</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G154" s="35" t="s">
         <v>53</v>
@@ -5417,7 +5417,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5432,10 +5432,10 @@
         <v>MDD</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F155" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G155" s="49" t="s">
         <v>93</v>
@@ -5443,7 +5443,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B156" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5458,10 +5458,10 @@
         <v>MDD</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G156" s="35" t="s">
         <v>55</v>
@@ -5469,7 +5469,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5484,10 +5484,10 @@
         <v>MOL</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G157" s="35" t="s">
         <v>56</v>
@@ -5510,10 +5510,10 @@
         <v>MOL</v>
       </c>
       <c r="E158" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F158" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G158" s="29" t="s">
         <v>56</v>
@@ -5521,7 +5521,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B159" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5536,18 +5536,18 @@
         <v>MPD</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G159" s="35" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="24" t="s">
-        <v>110</v>
+      <c r="A160" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B160" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5562,10 +5562,10 @@
         <v>SPF</v>
       </c>
       <c r="E160" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F160" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G160" s="34" t="s">
         <v>57</v>
@@ -5573,7 +5573,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B161" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5588,10 +5588,10 @@
         <v>SPF</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G161" s="35" t="s">
         <v>57</v>
@@ -5614,18 +5614,18 @@
         <v>SPF</v>
       </c>
       <c r="E162" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F162" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G162" s="29" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A163" s="24" t="s">
-        <v>110</v>
+      <c r="A163" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B163" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5640,10 +5640,10 @@
         <v>DEF</v>
       </c>
       <c r="E163" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G163" s="34" t="s">
         <v>32</v>
@@ -5651,7 +5651,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B164" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5666,10 +5666,10 @@
         <v>DEF</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G164" s="36" t="s">
         <v>32</v>
@@ -5692,10 +5692,10 @@
         <v>DEF</v>
       </c>
       <c r="E165" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F165" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G165" s="29" t="s">
         <v>32</v>
@@ -5703,7 +5703,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B166" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5718,18 +5718,18 @@
         <v>DWS</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G166" s="36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="24" t="s">
-        <v>110</v>
+      <c r="A167" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B167" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5744,18 +5744,18 @@
         <v>FWS</v>
       </c>
       <c r="E167" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G167" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B168" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5770,10 +5770,10 @@
         <v>LPF</v>
       </c>
       <c r="E168" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G168" s="35" t="s">
         <v>70</v>
@@ -5781,7 +5781,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B169" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5796,10 +5796,10 @@
         <v>LPF</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G169" s="36" t="s">
         <v>70</v>
@@ -5822,10 +5822,10 @@
         <v>LPF</v>
       </c>
       <c r="E170" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F170" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G170" s="29" t="s">
         <v>70</v>
@@ -5833,7 +5833,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B171" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5848,18 +5848,18 @@
         <v>MCF</v>
       </c>
       <c r="E171" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G171" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B172" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5874,18 +5874,18 @@
         <v>MPD</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G172" s="39" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A173" s="24" t="s">
-        <v>110</v>
+      <c r="A173" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B173" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5900,10 +5900,10 @@
         <v>SPF</v>
       </c>
       <c r="E173" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G173" s="34" t="s">
         <v>71</v>
@@ -5911,7 +5911,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B174" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5926,10 +5926,10 @@
         <v>SPF</v>
       </c>
       <c r="E174" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G174" s="35" t="s">
         <v>72</v>
@@ -5937,7 +5937,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B175" s="1" t="str">
         <f t="shared" si="13"/>
@@ -5952,10 +5952,10 @@
         <v>SPF</v>
       </c>
       <c r="E175" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G175" s="36" t="s">
         <v>71</v>
@@ -5978,10 +5978,10 @@
         <v>SPF</v>
       </c>
       <c r="E176" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F176" s="52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G176" s="31" t="s">
         <v>71</v>
@@ -5989,14 +5989,14 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B177" s="4" t="str">
         <f t="shared" ref="B177:B185" si="16">LEFT(G177,7)</f>
         <v>OTT_CRU</v>
       </c>
       <c r="C177" s="4" t="str">
-        <f t="shared" ref="C177:C208" si="17">LEFT(B177,3)</f>
+        <f t="shared" ref="C177:C185" si="17">LEFT(B177,3)</f>
         <v>OTT</v>
       </c>
       <c r="D177" s="4" t="str">
@@ -6004,10 +6004,10 @@
         <v>CRU</v>
       </c>
       <c r="E177" s="65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F177" s="65" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G177" s="73" t="s">
         <v>58</v>
@@ -6030,18 +6030,18 @@
         <v>CRU</v>
       </c>
       <c r="E178" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F178" s="42" t="s">
         <v>172</v>
-      </c>
-      <c r="F178" s="42" t="s">
-        <v>173</v>
       </c>
       <c r="G178" s="29" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A179" s="24" t="s">
-        <v>110</v>
+      <c r="A179" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B179" s="1" t="str">
         <f t="shared" si="16"/>
@@ -6056,10 +6056,10 @@
         <v>DEF</v>
       </c>
       <c r="E179" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G179" s="34" t="s">
         <v>33</v>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B180" s="1" t="str">
         <f t="shared" si="16"/>
@@ -6082,10 +6082,10 @@
         <v>DEF</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G180" s="35" t="s">
         <v>33</v>
@@ -6108,10 +6108,10 @@
         <v>DEF</v>
       </c>
       <c r="E181" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F181" s="42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G181" s="29" t="s">
         <v>33</v>
@@ -6119,7 +6119,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B182" s="1" t="str">
         <f t="shared" si="16"/>
@@ -6134,10 +6134,10 @@
         <v>DWS</v>
       </c>
       <c r="E182" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G182" s="35" t="s">
         <v>59</v>
@@ -6160,18 +6160,18 @@
         <v>MCD</v>
       </c>
       <c r="E183" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F183" s="42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G183" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B184" s="1" t="str">
         <f t="shared" si="16"/>
@@ -6186,10 +6186,10 @@
         <v>MOL</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G184" s="35" t="s">
         <v>60</v>
@@ -6212,10 +6212,10 @@
         <v>MOL</v>
       </c>
       <c r="E185" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F185" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G185" s="29" t="s">
         <v>61</v>
@@ -6223,69 +6223,69 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E186" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G186" s="36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E187" s="42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F187" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G187" s="43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D188" s="1" t="str">
         <f>RIGHT(B188,3)</f>
         <v>LPF</v>
       </c>
       <c r="E188" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F188" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G188" s="29" t="s">
         <v>95</v>
@@ -6293,94 +6293,94 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G189" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A190" s="24" t="s">
-        <v>110</v>
+      <c r="A190" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E190" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G190" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E191" s="42" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F191" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G191" s="43" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G192" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -6388,27 +6388,27 @@
         <v>1</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E193" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F193" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G193" s="29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B194" s="1" t="str">
         <f t="shared" ref="B194:B214" si="19">LEFT(G194,7)</f>
@@ -6423,10 +6423,10 @@
         <v>CRU</v>
       </c>
       <c r="E194" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G194" s="35" t="s">
         <v>62</v>
@@ -6449,18 +6449,18 @@
         <v>CRU</v>
       </c>
       <c r="E195" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F195" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G195" s="29" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A196" s="24" t="s">
-        <v>110</v>
+      <c r="A196" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B196" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6475,10 +6475,10 @@
         <v>DEF</v>
       </c>
       <c r="E196" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G196" s="34" t="s">
         <v>35</v>
@@ -6486,7 +6486,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B197" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6501,10 +6501,10 @@
         <v>DEF</v>
       </c>
       <c r="E197" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G197" s="35" t="s">
         <v>35</v>
@@ -6527,18 +6527,18 @@
         <v>DEF</v>
       </c>
       <c r="E198" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F198" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G198" s="29" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A199" s="24" t="s">
-        <v>110</v>
+      <c r="A199" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B199" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6553,18 +6553,18 @@
         <v>FWS</v>
       </c>
       <c r="E199" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G199" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B200" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6579,18 +6579,18 @@
         <v>MPD</v>
       </c>
       <c r="E200" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F200" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G200" s="35" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A201" s="24" t="s">
-        <v>110</v>
+      <c r="A201" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B201" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6605,10 +6605,10 @@
         <v>SPF</v>
       </c>
       <c r="E201" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G201" s="34" t="s">
         <v>65</v>
@@ -6616,7 +6616,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B202" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6631,10 +6631,10 @@
         <v>SPF</v>
       </c>
       <c r="E202" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F202" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G202" s="36" t="s">
         <v>65</v>
@@ -6657,18 +6657,18 @@
         <v>SPF</v>
       </c>
       <c r="E203" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F203" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G203" s="29" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A204" s="24" t="s">
-        <v>110</v>
+      <c r="A204" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B204" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6683,10 +6683,10 @@
         <v>DEF</v>
       </c>
       <c r="E204" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G204" s="34" t="s">
         <v>36</v>
@@ -6694,7 +6694,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B205" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6709,10 +6709,10 @@
         <v>DEF</v>
       </c>
       <c r="E205" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F205" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G205" s="36" t="s">
         <v>36</v>
@@ -6735,18 +6735,18 @@
         <v>DEF</v>
       </c>
       <c r="E206" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F206" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G206" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A207" s="24" t="s">
-        <v>110</v>
+      <c r="A207" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B207" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6761,18 +6761,18 @@
         <v>FWS</v>
       </c>
       <c r="E207" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F207" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G207" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B208" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6787,10 +6787,10 @@
         <v>LPF</v>
       </c>
       <c r="E208" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F208" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G208" s="35" t="s">
         <v>74</v>
@@ -6798,7 +6798,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B209" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6813,10 +6813,10 @@
         <v>LPF</v>
       </c>
       <c r="E209" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F209" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G209" s="36" t="s">
         <v>73</v>
@@ -6839,18 +6839,18 @@
         <v>LPF</v>
       </c>
       <c r="E210" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F210" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G210" s="29" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A211" s="24" t="s">
-        <v>110</v>
+      <c r="A211" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B211" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6865,10 +6865,10 @@
         <v>SPF</v>
       </c>
       <c r="E211" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G211" s="34" t="s">
         <v>75</v>
@@ -6876,7 +6876,7 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B212" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6891,10 +6891,10 @@
         <v>SPF</v>
       </c>
       <c r="E212" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F212" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G212" s="39" t="s">
         <v>96</v>
@@ -6902,7 +6902,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B213" s="1" t="str">
         <f t="shared" si="19"/>
@@ -6917,10 +6917,10 @@
         <v>SPF</v>
       </c>
       <c r="E213" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F213" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G213" s="36" t="s">
         <v>75</v>
@@ -6943,33 +6943,33 @@
         <v>SPF</v>
       </c>
       <c r="E214" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F214" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G214" s="29" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A215" s="24" t="s">
-        <v>110</v>
+      <c r="A215" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E215" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F215" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G215" s="40" t="s">
         <v>37</v>
@@ -6977,22 +6977,22 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E216" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F216" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G216" s="48" t="s">
         <v>37</v>
@@ -7000,22 +7000,22 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E217" s="56" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F217" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G217" s="57" t="s">
         <v>37</v>
@@ -7026,27 +7026,27 @@
         <v>1</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E218" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F218" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G218" s="48" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A219" s="24" t="s">
-        <v>110</v>
+      <c r="A219" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B219" s="1" t="str">
         <f t="shared" ref="B219:B226" si="22">LEFT(G219,7)</f>
@@ -7061,10 +7061,10 @@
         <v>DEF</v>
       </c>
       <c r="E219" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F219" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G219" s="34" t="s">
         <v>38</v>
@@ -7072,7 +7072,7 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B220" s="1" t="str">
         <f t="shared" si="22"/>
@@ -7087,10 +7087,10 @@
         <v>DEF</v>
       </c>
       <c r="E220" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F220" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G220" s="36" t="s">
         <v>38</v>
@@ -7113,10 +7113,10 @@
         <v>DEF</v>
       </c>
       <c r="E221" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F221" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G221" s="29" t="s">
         <v>38</v>
@@ -7124,7 +7124,7 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B222" s="1" t="str">
         <f t="shared" si="22"/>
@@ -7139,18 +7139,18 @@
         <v>MCF</v>
       </c>
       <c r="E222" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F222" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G222" s="36" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A223" s="24" t="s">
-        <v>110</v>
+      <c r="A223" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B223" s="1" t="str">
         <f t="shared" si="22"/>
@@ -7165,10 +7165,10 @@
         <v>DEF</v>
       </c>
       <c r="E223" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F223" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G223" s="34" t="s">
         <v>39</v>
@@ -7176,7 +7176,7 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B224" s="1" t="str">
         <f t="shared" si="22"/>
@@ -7191,10 +7191,10 @@
         <v>DEF</v>
       </c>
       <c r="E224" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F224" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G224" s="36" t="s">
         <v>39</v>
@@ -7217,18 +7217,18 @@
         <v>DEF</v>
       </c>
       <c r="E225" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F225" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G225" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A226" s="24" t="s">
-        <v>110</v>
+      <c r="A226" s="23" t="s">
+        <v>212</v>
       </c>
       <c r="B226" s="1" t="str">
         <f t="shared" si="22"/>
@@ -7243,33 +7243,33 @@
         <v>FWS</v>
       </c>
       <c r="E226" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F226" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G226" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F227" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G227" s="48" t="s">
         <v>97</v>
@@ -7277,7 +7277,7 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B228" s="1" t="str">
         <f t="shared" ref="B228:B235" si="25">LEFT(G228,7)</f>
@@ -7292,10 +7292,10 @@
         <v>CRU</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F228" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G228" s="36" t="s">
         <v>67</v>
@@ -7318,10 +7318,10 @@
         <v>CRU</v>
       </c>
       <c r="E229" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F229" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G229" s="29" t="s">
         <v>67</v>
@@ -7329,7 +7329,7 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B230" s="1" t="str">
         <f t="shared" si="25"/>
@@ -7344,10 +7344,10 @@
         <v>DEF</v>
       </c>
       <c r="E230" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F230" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G230" s="49" t="s">
         <v>98</v>
@@ -7355,7 +7355,7 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B231" s="1" t="str">
         <f t="shared" si="25"/>
@@ -7370,10 +7370,10 @@
         <v>DEF</v>
       </c>
       <c r="E231" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F231" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G231" s="36" t="s">
         <v>40</v>
@@ -7396,10 +7396,10 @@
         <v>DEF</v>
       </c>
       <c r="E232" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F232" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G232" s="29" t="s">
         <v>40</v>
@@ -7422,18 +7422,18 @@
         <v>MCD</v>
       </c>
       <c r="E233" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F233" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G233" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B234" s="1" t="str">
         <f t="shared" si="25"/>
@@ -7448,10 +7448,10 @@
         <v>MOL</v>
       </c>
       <c r="E234" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F234" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G234" s="36" t="s">
         <v>68</v>
@@ -7474,10 +7474,10 @@
         <v>MOL</v>
       </c>
       <c r="E235" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F235" s="52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G235" s="31" t="s">
         <v>69</v>

</xml_diff>